<commit_message>
0 in place of unused bioenergetic params, added in-built b consumed plot
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_221216.xlsx
+++ b/data/hake_intrasp_221216.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5937B28A-23D6-784E-B400-1FD3C6E038D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB65665F-EED4-6C40-94A6-6B4B8277AEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" firstSheet="7" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" firstSheet="5" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1908,7 +1908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="B28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -12015,8 +12015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12114,7 +12114,7 @@
         <v>153</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -12122,7 +12122,7 @@
         <v>154</v>
       </c>
       <c r="B13">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -12477,7 +12477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:R41"/>
     </sheetView>
   </sheetViews>
@@ -14969,7 +14969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>